<commit_message>
Fill more data for testing
</commit_message>
<xml_diff>
--- a/data/accounts.xlsx
+++ b/data/accounts.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Test Company 001</t>
+          <t>Acme Corporation</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -485,18 +485,20 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>zjbird@gmail.com</t>
+          <t>zjbird@gmail.com, jbubis@bestline.net, joshbubis@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test Company 002</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>53749</v>
+          <t>Beta Industries</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>53749, 98765</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -511,7 +513,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Test Company 003</t>
+          <t>Gamma Solutions</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -530,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Test Company 004</t>
+          <t>Delta Enterprises</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -549,11 +551,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Test Company 005</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>82753</v>
+          <t>Echo Technologies</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>82753, 54321</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -568,7 +572,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Test Company 006</t>
+          <t>Foxtrot Systems</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -587,7 +591,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Test Company 007</t>
+          <t>Golf Services</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -606,11 +610,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Test Company 008</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>80183</v>
+          <t>Hotel Group</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>80183, 11111</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -625,7 +631,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Test Company 009</t>
+          <t>India Corp</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -644,11 +650,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Test Company 010</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>54185</v>
+          <t>Juliet Business</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>54185, 99999</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -663,7 +671,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Test Company 011</t>
+          <t>Company 11</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -682,7 +690,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Test Company 012</t>
+          <t>Company 12</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -701,7 +709,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Test Company 013</t>
+          <t>Company 13</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -720,7 +728,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Test Company 014</t>
+          <t>Company 14</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -739,7 +747,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Test Company 015</t>
+          <t>Company 15</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -758,7 +766,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Test Company 016</t>
+          <t>Company 16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -777,7 +785,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Test Company 017</t>
+          <t>Company 17</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -796,7 +804,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Test Company 018</t>
+          <t>Company 18</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -815,7 +823,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Test Company 019</t>
+          <t>Company 19</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -834,7 +842,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Test Company 020</t>
+          <t>Company 20</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -853,7 +861,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Test Company 021</t>
+          <t>Company 21</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -872,7 +880,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Test Company 022</t>
+          <t>Company 22</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -891,7 +899,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Test Company 023</t>
+          <t>Company 23</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -910,7 +918,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Test Company 024</t>
+          <t>Company 24</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -929,7 +937,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Test Company 025</t>
+          <t>Company 25</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -948,7 +956,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Test Company 026</t>
+          <t>Company 26</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -967,7 +975,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Test Company 027</t>
+          <t>Company 27</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -986,7 +994,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Test Company 028</t>
+          <t>Company 28</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1005,7 +1013,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Test Company 029</t>
+          <t>Company 29</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1024,7 +1032,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Test Company 030</t>
+          <t>Company 30</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1043,7 +1051,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Test Company 031</t>
+          <t>Company 31</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1062,7 +1070,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Test Company 032</t>
+          <t>Company 32</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1081,7 +1089,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Test Company 033</t>
+          <t>Company 33</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1100,7 +1108,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Test Company 034</t>
+          <t>Company 34</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1119,7 +1127,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Test Company 035</t>
+          <t>Company 35</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1138,7 +1146,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Test Company 036</t>
+          <t>Company 36</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1157,7 +1165,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Test Company 037</t>
+          <t>Company 37</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1176,7 +1184,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Test Company 038</t>
+          <t>Company 38</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1195,7 +1203,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Test Company 039</t>
+          <t>Company 39</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1214,7 +1222,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Test Company 040</t>
+          <t>Company 40</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1233,7 +1241,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Test Company 041</t>
+          <t>Company 41</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1252,7 +1260,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Test Company 042</t>
+          <t>Company 42</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1271,7 +1279,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Test Company 043</t>
+          <t>Company 43</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1290,7 +1298,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Test Company 044</t>
+          <t>Company 44</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1309,7 +1317,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Test Company 045</t>
+          <t>Company 45</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1328,7 +1336,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Test Company 046</t>
+          <t>Company 46</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1347,7 +1355,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Test Company 047</t>
+          <t>Company 47</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1366,7 +1374,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Test Company 048</t>
+          <t>Company 48</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1385,7 +1393,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Test Company 049</t>
+          <t>Company 49</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1404,7 +1412,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Test Company 050</t>
+          <t>Company 50</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1423,7 +1431,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Test Company 051</t>
+          <t>Company 51</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1442,7 +1450,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Test Company 052</t>
+          <t>Company 52</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1461,7 +1469,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Test Company 053</t>
+          <t>Company 53</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1480,7 +1488,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Test Company 054</t>
+          <t>Company 54</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1499,7 +1507,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Test Company 055</t>
+          <t>Company 55</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1518,7 +1526,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Test Company 056</t>
+          <t>Company 56</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1537,7 +1545,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Test Company 057</t>
+          <t>Company 57</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1556,7 +1564,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Test Company 058</t>
+          <t>Company 58</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1575,7 +1583,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Test Company 059</t>
+          <t>Company 59</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1594,7 +1602,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Test Company 060</t>
+          <t>Company 60</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1613,7 +1621,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Test Company 061</t>
+          <t>Company 61</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1632,7 +1640,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Test Company 062</t>
+          <t>Company 62</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1651,7 +1659,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Test Company 063</t>
+          <t>Company 63</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1670,7 +1678,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Test Company 064</t>
+          <t>Company 64</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1689,7 +1697,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Test Company 065</t>
+          <t>Company 65</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1708,7 +1716,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Test Company 066</t>
+          <t>Company 66</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1727,7 +1735,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Test Company 067</t>
+          <t>Company 67</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1746,7 +1754,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Test Company 068</t>
+          <t>Company 68</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1765,7 +1773,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Test Company 069</t>
+          <t>Company 69</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1784,7 +1792,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Test Company 070</t>
+          <t>Company 70</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1803,7 +1811,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Test Company 071</t>
+          <t>Company 71</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1822,7 +1830,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Test Company 072</t>
+          <t>Company 72</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1841,7 +1849,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Test Company 073</t>
+          <t>Company 73</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1860,7 +1868,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Test Company 074</t>
+          <t>Company 74</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1879,7 +1887,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Test Company 075</t>
+          <t>Company 75</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1898,7 +1906,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Test Company 076</t>
+          <t>Company 76</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1917,7 +1925,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Test Company 077</t>
+          <t>Company 77</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1936,7 +1944,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Test Company 078</t>
+          <t>Company 78</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1955,7 +1963,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Test Company 079</t>
+          <t>Company 79</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1974,7 +1982,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Test Company 080</t>
+          <t>Company 80</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1993,7 +2001,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Test Company 081</t>
+          <t>Company 81</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2012,7 +2020,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Test Company 082</t>
+          <t>Company 82</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -2031,7 +2039,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Test Company 083</t>
+          <t>Company 83</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -2050,7 +2058,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Test Company 084</t>
+          <t>Company 84</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -2069,7 +2077,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Test Company 085</t>
+          <t>Company 85</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -2088,7 +2096,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Test Company 086</t>
+          <t>Company 86</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -2107,7 +2115,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Test Company 087</t>
+          <t>Company 87</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -2126,7 +2134,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Test Company 088</t>
+          <t>Company 88</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -2145,7 +2153,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Test Company 089</t>
+          <t>Company 89</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -2164,7 +2172,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Test Company 090</t>
+          <t>Company 90</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -2183,7 +2191,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Test Company 091</t>
+          <t>Company 91</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -2202,7 +2210,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Test Company 092</t>
+          <t>Company 92</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -2221,7 +2229,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Test Company 093</t>
+          <t>Company 93</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -2240,7 +2248,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Test Company 094</t>
+          <t>Company 94</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2259,7 +2267,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Test Company 095</t>
+          <t>Company 95</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -2278,7 +2286,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Test Company 096</t>
+          <t>Company 96</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -2297,7 +2305,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Test Company 097</t>
+          <t>Company 97</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -2316,7 +2324,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Test Company 098</t>
+          <t>Company 98</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -2335,7 +2343,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Test Company 099</t>
+          <t>Company 99</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -2354,7 +2362,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Test Company 100</t>
+          <t>Company 100</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -2373,7 +2381,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Test Company 89600</t>
+          <t>Company 101</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -2392,7 +2400,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Test Company 83458</t>
+          <t>Company 102</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -2411,7 +2419,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Test Company 72708</t>
+          <t>Company 103</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -2430,7 +2438,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Test Company 36869</t>
+          <t>Company 104</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -2449,7 +2457,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Test Company 49159</t>
+          <t>Company 105</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -2468,7 +2476,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Test Company 47640</t>
+          <t>Company 106</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -2487,7 +2495,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Test Company 98329</t>
+          <t>Company 107</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -2506,7 +2514,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Test Company 63008</t>
+          <t>Company 108</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -2525,7 +2533,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Test Company 22562</t>
+          <t>Company 109</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -2544,7 +2552,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Test Company 96803</t>
+          <t>Company 110</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -2563,7 +2571,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Test Company 93220</t>
+          <t>Company 111</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -2582,7 +2590,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Test Company 72226</t>
+          <t>Company 112</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -2601,7 +2609,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Test Company 16937</t>
+          <t>Company 113</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -2620,7 +2628,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Test Company 42542</t>
+          <t>Company 114</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -2639,7 +2647,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Test Company 60975</t>
+          <t>Company 115</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -2658,7 +2666,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Test Company 73783</t>
+          <t>Company 116</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -2677,7 +2685,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Test Company 47674</t>
+          <t>Company 117</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -2696,7 +2704,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Test Company 63039</t>
+          <t>Company 118</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -2715,7 +2723,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Test Company 50240</t>
+          <t>Company 119</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -2734,7 +2742,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Test Company 61524</t>
+          <t>Company 120</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -2753,7 +2761,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Test Company 97364</t>
+          <t>Company 121</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -2772,7 +2780,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Test Company 82009</t>
+          <t>Company 122</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -2791,7 +2799,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Test Company 78938</t>
+          <t>Company 123</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -2810,7 +2818,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Test Company 43099</t>
+          <t>Company 124</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -2829,7 +2837,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Test Company 75356</t>
+          <t>Company 125</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2848,7 +2856,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Test Company 96867</t>
+          <t>Company 126</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -2867,7 +2875,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Test Company 47206</t>
+          <t>Company 127</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2886,7 +2894,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Test Company 76396</t>
+          <t>Company 128</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -2905,7 +2913,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Test Company 15983</t>
+          <t>Company 129</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -2924,7 +2932,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Test Company 44656</t>
+          <t>Company 130</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -2943,7 +2951,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Test Company 68719</t>
+          <t>Company 131</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -2962,7 +2970,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Test Company 92275</t>
+          <t>Company 132</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -2981,7 +2989,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Test Company 76916</t>
+          <t>Company 133</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -3000,7 +3008,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Test Company 23156</t>
+          <t>Company 134</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -3019,7 +3027,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Test Company 49270</t>
+          <t>Company 135</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -3038,7 +3046,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Test Company 50293</t>
+          <t>Company 136</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -3057,7 +3065,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Test Company 71288</t>
+          <t>Company 137</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -3076,7 +3084,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Test Company 95350</t>
+          <t>Company 138</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -3095,7 +3103,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Test Company 82556</t>
+          <t>Company 139</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -3114,7 +3122,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Test Company 99452</t>
+          <t>Company 140</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -3133,7 +3141,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Test Company 18561</t>
+          <t>Company 141</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -3152,7 +3160,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Test Company 90757</t>
+          <t>Company 142</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -3171,7 +3179,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Test Company 27272</t>
+          <t>Company 143</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -3190,7 +3198,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Test Company 56968</t>
+          <t>Company 144</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -3209,7 +3217,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Test Company 50315</t>
+          <t>Company 145</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -3228,7 +3236,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Test Company 80525</t>
+          <t>Company 146</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -3247,7 +3255,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Test Company 95374</t>
+          <t>Company 147</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -3266,7 +3274,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Test Company 35470</t>
+          <t>Company 148</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -3285,7 +3293,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Test Company 72850</t>
+          <t>Company 149</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -3304,7 +3312,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Test Company 74392</t>
+          <t>Company 150</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -3323,7 +3331,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Test Company 53425</t>
+          <t>Company 151</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -3342,7 +3350,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Test Company 19635</t>
+          <t>Company 152</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -3361,7 +3369,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Test Company 29364</t>
+          <t>Company 153</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -3380,7 +3388,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Test Company 23221</t>
+          <t>Company 154</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -3399,7 +3407,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Test Company 74419</t>
+          <t>Company 155</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -3418,7 +3426,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Test Company 37566</t>
+          <t>Company 156</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -3437,7 +3445,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Test Company 55998</t>
+          <t>Company 157</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -3456,7 +3464,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Test Company 39104</t>
+          <t>Company 158</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -3475,7 +3483,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Test Company 63172</t>
+          <t>Company 159</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -3494,7 +3502,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Test Company 94917</t>
+          <t>Company 160</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -3513,7 +3521,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Test Company 99525</t>
+          <t>Company 161</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -3532,7 +3540,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Test Company 17611</t>
+          <t>Company 162</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -3551,7 +3559,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Test Company 66763</t>
+          <t>Company 163</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -3570,7 +3578,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Test Company 77005</t>
+          <t>Company 164</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -3589,7 +3597,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Test Company 11470</t>
+          <t>Company 165</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -3608,7 +3616,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Test Company 15055</t>
+          <t>Company 166</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -3627,7 +3635,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Test Company 40657</t>
+          <t>Company 167</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -3646,7 +3654,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Test Company 34514</t>
+          <t>Company 168</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -3665,7 +3673,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Test Company 22742</t>
+          <t>Company 169</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -3684,7 +3692,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Test Company 14038</t>
+          <t>Company 170</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -3703,7 +3711,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Test Company 11480</t>
+          <t>Company 171</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -3722,7 +3730,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Test Company 34008</t>
+          <t>Company 172</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -3741,7 +3749,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Test Company 66266</t>
+          <t>Company 173</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -3760,7 +3768,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Test Company 63202</t>
+          <t>Company 174</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -3779,7 +3787,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Test Company 16614</t>
+          <t>Company 175</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -3798,7 +3806,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Test Company 61160</t>
+          <t>Company 176</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -3817,7 +3825,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Test Company 65270</t>
+          <t>Company 177</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -3836,7 +3844,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Test Company 97527</t>
+          <t>Company 178</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -3855,7 +3863,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Test Company 39160</t>
+          <t>Company 179</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -3874,7 +3882,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Test Company 57593</t>
+          <t>Company 180</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -3893,7 +3901,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Test Company 95482</t>
+          <t>Company 181</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -3912,7 +3920,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Test Company 10494</t>
+          <t>Company 182</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -3931,7 +3939,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Test Company 67329</t>
+          <t>Company 183</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -3950,7 +3958,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Test Company 70402</t>
+          <t>Company 184</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -3969,7 +3977,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Test Company 73476</t>
+          <t>Company 185</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -3988,7 +3996,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Test Company 63756</t>
+          <t>Company 186</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -4007,7 +4015,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Test Company 47893</t>
+          <t>Company 187</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -4026,7 +4034,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Test Company 85784</t>
+          <t>Company 188</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -4045,7 +4053,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Test Company 89883</t>
+          <t>Company 189</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -4064,7 +4072,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Test Company 41246</t>
+          <t>Company 190</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -4083,7 +4091,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Test Company 79139</t>
+          <t>Company 191</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -4102,7 +4110,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Test Company 87845</t>
+          <t>Company 192</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -4121,7 +4129,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Test Company 31528</t>
+          <t>Company 193</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -4140,7 +4148,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Test Company 15659</t>
+          <t>Company 194</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -4159,7 +4167,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Test Company 46379</t>
+          <t>Company 195</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -4178,7 +4186,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Test Company 71982</t>
+          <t>Company 196</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -4197,7 +4205,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Test Company 71992</t>
+          <t>Company 197</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -4216,7 +4224,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Test Company 54074</t>
+          <t>Company 198</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -4235,7 +4243,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Test Company 31550</t>
+          <t>Company 199</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -4254,7 +4262,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Test Company 94014</t>
+          <t>Company 200</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -4273,7 +4281,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Test Company 75071</t>
+          <t>Company 201</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -4292,7 +4300,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Test Company 75589</t>
+          <t>Company 202</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -4311,7 +4319,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Test Company 35659</t>
+          <t>Company 203</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -4330,7 +4338,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Test Company 16205</t>
+          <t>Company 204</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -4349,7 +4357,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Test Company 53584</t>
+          <t>Company 205</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -4368,7 +4376,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Test Company 42327</t>
+          <t>Company 206</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -4387,7 +4395,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Test Company 72535</t>
+          <t>Company 207</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -4406,7 +4414,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Test Company 46937</t>
+          <t>Company 208</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -4425,7 +4433,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Test Company 35162</t>
+          <t>Company 209</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -4444,7 +4452,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Test Company 26972</t>
+          <t>Company 210</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -4463,7 +4471,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Test Company 39269</t>
+          <t>Company 211</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -4482,7 +4490,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Test Company 69479</t>
+          <t>Company 212</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -4501,7 +4509,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Test Company 42859</t>
+          <t>Company 213</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -4520,7 +4528,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Test Company 44908</t>
+          <t>Company 214</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -4539,7 +4547,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Test Company 38254</t>
+          <t>Company 215</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -4558,7 +4566,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Test Company 22896</t>
+          <t>Company 216</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -4577,7 +4585,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Test Company 70005</t>
+          <t>Company 217</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -4596,7 +4604,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Test Company 44407</t>
+          <t>Company 218</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -4615,7 +4623,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Test Company 43905</t>
+          <t>Company 219</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -4634,7 +4642,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Test Company 14209</t>
+          <t>Company 220</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -4653,7 +4661,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Test Company 96644</t>
+          <t>Company 221</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -4672,7 +4680,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Test Company 75142</t>
+          <t>Company 222</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -4691,7 +4699,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Test Company 96134</t>
+          <t>Company 223</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -4710,7 +4718,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Test Company 40841</t>
+          <t>Company 224</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -4729,7 +4737,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Test Company 76171</t>
+          <t>Company 225</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -4748,7 +4756,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Test Company 69004</t>
+          <t>Company 226</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -4767,7 +4775,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Test Company 24461</t>
+          <t>Company 227</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -4786,7 +4794,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Test Company 43408</t>
+          <t>Company 228</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -4805,7 +4813,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Test Company 40856</t>
+          <t>Company 229</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -4824,7 +4832,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Test Company 82330</t>
+          <t>Company 230</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -4843,7 +4851,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Test Company 55202</t>
+          <t>Company 231</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -4862,7 +4870,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Test Company 38307</t>
+          <t>Company 232</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -4881,7 +4889,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Test Company 63908</t>
+          <t>Company 233</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -4900,7 +4908,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Test Company 18856</t>
+          <t>Company 234</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -4919,7 +4927,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Test Company 26537</t>
+          <t>Company 235</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -4938,7 +4946,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Test Company 50093</t>
+          <t>Company 236</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -4957,7 +4965,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Test Company 57777</t>
+          <t>Company 237</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -4976,7 +4984,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Test Company 20407</t>
+          <t>Company 238</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -4995,7 +5003,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Test Company 17849</t>
+          <t>Company 239</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -5014,7 +5022,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Test Company 38842</t>
+          <t>Company 240</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -5033,7 +5041,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Test Company 78782</t>
+          <t>Company 241</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -5052,7 +5060,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Test Company 86464</t>
+          <t>Company 242</t>
         </is>
       </c>
       <c r="B243" t="n">
@@ -5071,7 +5079,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Test Company 93634</t>
+          <t>Company 243</t>
         </is>
       </c>
       <c r="B244" t="n">
@@ -5090,7 +5098,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Test Company 93636</t>
+          <t>Company 244</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -5109,7 +5117,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Test Company 67527</t>
+          <t>Company 245</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -5128,7 +5136,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Test Company 42441</t>
+          <t>Company 246</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -5147,7 +5155,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Test Company 65994</t>
+          <t>Company 247</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -5166,7 +5174,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Test Company 30155</t>
+          <t>Company 248</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -5185,7 +5193,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Test Company 43475</t>
+          <t>Company 249</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -5204,7 +5212,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Test Company 62931</t>
+          <t>Company 250</t>
         </is>
       </c>
       <c r="B251" t="n">
@@ -5223,7 +5231,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Test Company 28628</t>
+          <t>Company 251</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -5242,7 +5250,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Test Company 74198</t>
+          <t>Company 252</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -5261,7 +5269,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Test Company 61398</t>
+          <t>Company 253</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -5280,7 +5288,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Test Company 54239</t>
+          <t>Company 254</t>
         </is>
       </c>
       <c r="B255" t="n">
@@ -5299,7 +5307,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Test Company 59359</t>
+          <t>Company 255</t>
         </is>
       </c>
       <c r="B256" t="n">
@@ -5318,7 +5326,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Test Company 21478</t>
+          <t>Company 256</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -5337,7 +5345,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Test Company 17385</t>
+          <t>Company 257</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -5356,7 +5364,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Test Company 54763</t>
+          <t>Company 258</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -5375,7 +5383,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Test Company 63979</t>
+          <t>Company 259</t>
         </is>
       </c>
       <c r="B260" t="n">
@@ -5394,7 +5402,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Test Company 64493</t>
+          <t>Company 260</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -5413,7 +5421,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Test Company 55788</t>
+          <t>Company 261</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -5432,7 +5440,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Test Company 72688</t>
+          <t>Company 262</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -5451,7 +5459,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Test Company 32758</t>
+          <t>Company 263</t>
         </is>
       </c>
       <c r="B264" t="n">
@@ -5470,7 +5478,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Test Company 83450</t>
+          <t>Company 264</t>
         </is>
       </c>
       <c r="B265" t="n">
@@ -5489,7 +5497,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Test Company 83452</t>
+          <t>Company 265</t>
         </is>
       </c>
       <c r="B266" t="n">

</xml_diff>